<commit_message>
Corregidos errores de reporteo de asistencia. Mejorada funcionalidad de exportación a Excel. Modificación de templates de Excel. Refactorización de código en AsistenciasController.
</commit_message>
<xml_diff>
--- a/NOAM_ASISTENCIA_V2/Server/wwwroot/docs/NOAM_REPORTES_28.xlsx
+++ b/NOAM_ASISTENCIA_V2/Server/wwwroot/docs/NOAM_REPORTES_28.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\FIME\NOAM_ASISTENCIA_v2\NOAM_ASISTENCIA_V2\Server\wwwroot\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\FIME\NOAM_ASISTENCIA_v2\NOAM_ASISTENCIA_v2\Server\wwwroot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F740BE99-2460-46AD-B4E9-0EDAB4145536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32AAEB5-A008-4AE4-970C-AE4D3345CC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A26607A-8AD9-4F9E-A4BC-D55BA9D7932A}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,68 +474,81 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -911,7 +924,7 @@
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,141 +940,141 @@
     <col min="13" max="13" width="3" style="14" customWidth="1"/>
     <col min="14" max="31" width="3" style="14" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="3" style="15" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.33203125" style="43" customWidth="1"/>
-    <col min="34" max="35" width="10.6640625" style="43" customWidth="1"/>
+    <col min="33" max="33" width="10.33203125" style="31" customWidth="1"/>
+    <col min="34" max="35" width="10.6640625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="2" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="35" t="s">
+      <c r="A1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="27"/>
     </row>
     <row r="2" spans="1:35" s="2" customFormat="1" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="44" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="39"/>
-      <c r="AI2" s="39"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="42"/>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="42"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="42"/>
+      <c r="AF2" s="43"/>
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
     </row>
     <row r="3" spans="1:35" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="29"/>
-      <c r="AF3" s="30"/>
-      <c r="AG3" s="40"/>
-      <c r="AH3" s="40"/>
-      <c r="AI3" s="40"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="36"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29"/>
     </row>
     <row r="4" spans="1:35" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="33" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="9"/>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <v>1</v>
       </c>
       <c r="F4" s="25">
@@ -1145,9 +1158,9 @@
       <c r="AF4" s="25">
         <v>28</v>
       </c>
-      <c r="AG4" s="41"/>
-      <c r="AH4" s="41"/>
-      <c r="AI4" s="41"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="30"/>
     </row>
     <row r="5" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
@@ -1182,9 +1195,9 @@
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
       <c r="AF5" s="11"/>
-      <c r="AG5" s="42"/>
-      <c r="AH5" s="42"/>
-      <c r="AI5" s="42"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
     </row>
     <row r="6" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
@@ -1219,9 +1232,9 @@
       <c r="AD6" s="12"/>
       <c r="AE6" s="12"/>
       <c r="AF6" s="13"/>
-      <c r="AG6" s="42"/>
-      <c r="AH6" s="42"/>
-      <c r="AI6" s="42"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
     </row>
     <row r="7" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -1256,9 +1269,9 @@
       <c r="AD7" s="12"/>
       <c r="AE7" s="12"/>
       <c r="AF7" s="13"/>
-      <c r="AG7" s="42"/>
-      <c r="AH7" s="42"/>
-      <c r="AI7" s="42"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
     </row>
     <row r="8" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -1293,9 +1306,9 @@
       <c r="AD8" s="12"/>
       <c r="AE8" s="12"/>
       <c r="AF8" s="13"/>
-      <c r="AG8" s="42"/>
-      <c r="AH8" s="42"/>
-      <c r="AI8" s="42"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
     </row>
     <row r="9" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
@@ -1330,9 +1343,9 @@
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
       <c r="AF9" s="13"/>
-      <c r="AG9" s="42"/>
-      <c r="AH9" s="42"/>
-      <c r="AI9" s="42"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
     </row>
     <row r="10" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
@@ -1367,9 +1380,9 @@
       <c r="AD10" s="12"/>
       <c r="AE10" s="12"/>
       <c r="AF10" s="13"/>
-      <c r="AG10" s="42"/>
-      <c r="AH10" s="42"/>
-      <c r="AI10" s="42"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
     </row>
     <row r="11" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
@@ -1404,9 +1417,9 @@
       <c r="AD11" s="12"/>
       <c r="AE11" s="12"/>
       <c r="AF11" s="13"/>
-      <c r="AG11" s="42"/>
-      <c r="AH11" s="42"/>
-      <c r="AI11" s="42"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:C11" xr:uid="{F6B9F883-765B-4AC3-9155-BEA24AA6D9C4}"/>
@@ -1418,8 +1431,13 @@
     <mergeCell ref="C1:AF1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:AI1048576 E3 AG3:AI3">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",E3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:AF1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="·">
+      <formula>NOT(ISERROR(SEARCH("·",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>